<commit_message>
LE module status in settings (see description)
- Added a line under Astrophotography showing a status if le magisk module is installed.
- Slightly edited camera_preferences so there's no need for a separate input from strings.xml
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="55">
   <si>
     <t xml:space="preserve">Notes:</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">Astrophotography countdown fix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max exposure toast</t>
   </si>
 </sst>
 </file>
@@ -384,13 +387,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+      <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.06640625" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.21"/>
   </cols>
@@ -968,10 +971,30 @@
         <v>16</v>
       </c>
     </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
do not enable Tracking Focus for Pixel 1 by default
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1573427241" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1573427241" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1573427241" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1573427241"/>
+      <pm:revision xmlns:pm="smNativeData" day="1573440613" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1573440613" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1573440613" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1573440613"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="56">
   <si>
     <t>Notes:</t>
   </si>
@@ -220,7 +220,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -235,7 +235,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" fgClr="FF9900" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" fgClr="FF9900" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -251,7 +251,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" fgClr="999999" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" fgClr="999999" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="200" lang="default" i="1"/>
@@ -266,7 +266,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" fgClr="0070C0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" fgClr="0070C0" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -281,7 +281,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -303,7 +303,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1573427241" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1573440613" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -325,7 +325,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573427241"/>
+          <pm:border xmlns:pm="smNativeData" id="1573440613"/>
         </ext>
       </extLst>
     </border>
@@ -344,7 +344,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573427241"/>
+          <pm:border xmlns:pm="smNativeData" id="1573440613"/>
         </ext>
       </extLst>
     </border>
@@ -364,11 +364,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -381,10 +381,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1573427241" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1573440613" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1573427241" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1573440613" count="2">
         <pm:color name="Color 24" rgb="FF9900"/>
         <pm:color name="Color 25" rgb="0070C0"/>
       </pm:colors>
@@ -651,618 +651,625 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.081081" defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="37.207207" customWidth="1" style="6"/>
+    <col min="1" max="1" width="37.207207" customWidth="1" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="6" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="6" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="6" t="s">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="6" t="s">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="B11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="6" t="s">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="C12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="6" t="s">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="B13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="6" t="s">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="6" t="s">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="C15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="6" t="s">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="C16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="6" t="s">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="B17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="6" t="s">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="D18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="6" t="s">
+      <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="6" t="s">
+      <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="B20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="6" t="s">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="6" t="s">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="D22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="6" t="s">
+      <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="C23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="6" t="s">
+      <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="8" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="6" t="s">
+      <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="8" t="s">
+      <c r="B25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="6" t="s">
+      <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="6" t="s">
+      <c r="A27" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="6" t="s">
+      <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="9" t="s">
+      <c r="B28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="6" t="s">
+      <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="9" t="s">
+      <c r="B29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="6" t="s">
+      <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30" s="9" t="s">
+      <c r="B30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="6" t="s">
+      <c r="A31" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="9" t="s">
+      <c r="B31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="6" t="s">
+      <c r="A32" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="6" t="s">
+      <c r="A33" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="6" t="s">
+      <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" s="9" t="s">
+      <c r="B34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="6" t="s">
+      <c r="A35" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="6" t="s">
+      <c r="A36" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="6" t="s">
+      <c r="A37" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="6" t="s">
+      <c r="A38" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" s="9" t="s">
+      <c r="B38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="6" t="s">
+      <c r="A39" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F40" s="9" t="s">
+      <c r="B40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F41" s="9" t="s">
+      <c r="B41" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="6" t="s">
+      <c r="A42" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="B42" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E42" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F42" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="6" t="s">
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="B43" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="9" t="s">
+      <c r="B44" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F45" s="9" t="s">
+      <c r="B45" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="6" t="s">
+      <c r="A46" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1273,7 +1280,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573427241" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1573440613" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1282,16 +1289,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573427241" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573427241" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1573427241" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1573427241" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1573440613" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1573440613" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1573440613" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1573440613" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573427241" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573440613" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Revert "do not enable Tracking Focus for Pixel 1 by default"
This reverts commit c63be5040d4aa23c7219e53063963092d05d0b35.
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1573440613" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1573440613" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1573440613" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1573440613"/>
+      <pm:revision xmlns:pm="smNativeData" day="1573427241" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1573427241" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1573427241" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1573427241"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="56">
   <si>
     <t>Notes:</t>
   </si>
@@ -220,7 +220,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -235,7 +235,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" fgClr="FF9900" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" fgClr="FF9900" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -251,7 +251,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" fgClr="999999" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" fgClr="999999" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="200" lang="default" i="1"/>
@@ -266,7 +266,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" fgClr="0070C0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" fgClr="0070C0" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -281,7 +281,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573440613" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573427241" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -303,7 +303,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1573440613" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1573427241" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -325,7 +325,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573440613"/>
+          <pm:border xmlns:pm="smNativeData" id="1573427241"/>
         </ext>
       </extLst>
     </border>
@@ -344,7 +344,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573440613"/>
+          <pm:border xmlns:pm="smNativeData" id="1573427241"/>
         </ext>
       </extLst>
     </border>
@@ -364,11 +364,11 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -381,10 +381,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1573440613" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1573427241" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1573440613" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1573427241" count="2">
         <pm:color name="Color 24" rgb="FF9900"/>
         <pm:color name="Color 25" rgb="0070C0"/>
       </pm:colors>
@@ -651,625 +651,618 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.081081" defaultRowHeight="13.45"/>
   <cols>
-    <col min="1" max="1" width="37.207207" customWidth="1" style="0"/>
+    <col min="1" max="1" width="37.207207" customWidth="1" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="7" t="s">
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="C12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="7" t="s">
+      <c r="B13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="C14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
+      <c r="A15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="C15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" t="s">
+      <c r="A16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="7" t="s">
+      <c r="C16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="B17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" t="s">
+      <c r="A18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="7" t="s">
+      <c r="D18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="7" t="s">
+      <c r="B19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" t="s">
+      <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="7" t="s">
+      <c r="B20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" t="s">
+      <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" t="s">
+      <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="7" t="s">
+      <c r="D22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" t="s">
+      <c r="A23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="7" t="s">
+      <c r="C23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="7" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" t="s">
+      <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="B25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="A26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="A27" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" t="s">
+      <c r="A28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="8" t="s">
+      <c r="B28" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" s="8" t="s">
+      <c r="B29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" t="s">
+      <c r="A30" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F30" s="8" t="s">
+      <c r="B30" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" t="s">
+      <c r="A31" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="8" t="s">
+      <c r="B31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" t="s">
+      <c r="A32" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" t="s">
+      <c r="A33" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" t="s">
+      <c r="A34" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" s="8" t="s">
+      <c r="B34" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" t="s">
+      <c r="A35" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" t="s">
+      <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" t="s">
+      <c r="A37" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" t="s">
+      <c r="A38" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" s="8" t="s">
+      <c r="B38" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" t="s">
+      <c r="A39" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F40" s="8" t="s">
+      <c r="B40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F41" s="8" t="s">
+      <c r="B41" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" t="s">
+      <c r="A42" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="C42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
+    <row r="43" spans="1:2">
+      <c r="A43" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
+      <c r="B43" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="B44" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E44" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F45" s="8" t="s">
+      <c r="B45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" t="s">
+      <c r="A46" s="6" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1280,7 +1273,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573440613" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1573427241" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1289,16 +1282,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573440613" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573440613" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1573440613" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1573440613" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1573427241" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1573427241" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1573427241" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1573427241" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573440613" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573427241" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Enabled hevc for P1
Confirmed with MediaInfo.
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="57">
   <si>
     <t xml:space="preserve">Notes:</t>
   </si>
@@ -411,10 +411,10 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D49" activeCellId="0" sqref="D49"/>
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.09375" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.1015625" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.21"/>
   </cols>
@@ -511,13 +511,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
@@ -531,10 +529,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>18</v>
       </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
@@ -548,10 +549,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
@@ -565,9 +569,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
@@ -714,11 +721,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>13</v>
       </c>
@@ -1053,7 +1062,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="atEnd" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fixed P1 tracking focus for photo mode
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="57">
   <si>
     <t xml:space="preserve">Notes:</t>
   </si>
@@ -411,10 +411,10 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.1015625" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12109375" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.21"/>
   </cols>
@@ -666,11 +666,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Added 4K timelapse toggle
Default is set to 1080p, regardless of device.
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="57">
   <si>
     <t xml:space="preserve">Notes:</t>
   </si>
@@ -411,10 +411,10 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
+      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.12109375" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.21"/>
   </cols>
@@ -891,9 +891,24 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>45</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added force astro mode button (see desc)
Both force astro and light trails are enabled by a single toggle for now. I also haven't changed the toggle description yet, maybe we can finalize that after a few trials.
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="58">
   <si>
     <t xml:space="preserve">Notes:</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t xml:space="preserve">Need test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astrophotography always-on button</t>
   </si>
 </sst>
 </file>
@@ -408,13 +411,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+      <selection pane="topLeft" activeCell="H46" activeCellId="0" sqref="H46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.1484375" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.21"/>
   </cols>
@@ -1063,14 +1066,34 @@
       <c r="C46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>56</v>
+      <c r="D46" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add About section to prefs
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1573706553" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1573706553" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1573706553" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1573706553"/>
+      <pm:revision xmlns:pm="smNativeData" day="1573706848" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1573706848" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1573706848" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1573706848"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="57">
   <si>
     <t>Notes:</t>
   </si>
@@ -223,7 +223,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573706553" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573706848" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -238,7 +238,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573706553" fgClr="FF9900" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573706848" fgClr="FF9900" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -254,7 +254,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573706553" fgClr="999999" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573706848" fgClr="999999" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="200" lang="default" i="1"/>
@@ -269,7 +269,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573706553" fgClr="999999" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573706848" fgClr="999999" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -284,7 +284,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573706553" fgClr="0070C0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573706848" fgClr="0070C0" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -299,7 +299,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573706553" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1573706848" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -332,7 +332,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573706553"/>
+          <pm:border xmlns:pm="smNativeData" id="1573706848"/>
         </ext>
       </extLst>
     </border>
@@ -375,10 +375,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1573706553" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1573706848" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1573706553" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1573706848" count="2">
         <pm:color name="Color 24" rgb="FF9900"/>
         <pm:color name="Color 25" rgb="0070C0"/>
       </pm:colors>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.144144" defaultRowHeight="13.45"/>
@@ -1281,10 +1281,18 @@
       <c r="B43" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
+      <c r="C43" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="10" t="s">
@@ -1367,13 +1375,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B43:F43"/>
-  </mergeCells>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573706553" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1573706848" printRowHead="0" printColHead="0" printHeadLine="1" printFootLine="1" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1382,16 +1387,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573706553" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573706553" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1573706553" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1573706553" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1573706848" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1573706848" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1573706848" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1573706848" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573706553" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573706848" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Disable Portrait Touch Focus for 3a (crashes)
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camerons\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\APK+Easy+Tool+1.55+Portable\1-Decompiled APKs\PXv4_GoogleCamera_7.2.014\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DF8AC2-068D-4B03-84B8-7F5F22183AC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E82EE7-F94B-493F-8B00-DA38FD738A10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="1965" windowWidth="25275" windowHeight="13605" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="2310" windowWidth="25275" windowHeight="13605" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(_$* #,##0.00_);_(_$* \(#,##0.00\);_(_$* &quot;-&quot;????_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="_(_$* #,##0_);_(_$* \(#,##0\);_(_$* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;????_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(_$* #,##0.00_);_(_$* \(#,##0.00\);_(_$* &quot;-&quot;????_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(_$* #,##0_);_(_$* \(#,##0\);_(_$* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;????_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -281,9 +281,9 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="173" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="174" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -589,7 +589,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -902,8 +902,8 @@
       <c r="D23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>13</v>
+      <c r="E23" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
add info to astro max time toggle
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1573968809" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1573968809" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1573968809" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1573968809"/>
+      <pm:revision xmlns:pm="smNativeData" day="1574055446" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1574055446" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1574055446" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1574055446"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="62">
   <si>
     <t>Notes:</t>
   </si>
@@ -154,6 +154,9 @@
     <t>Exposure Slider</t>
   </si>
   <si>
+    <t>Not Working</t>
+  </si>
+  <si>
     <t>ISO Slider</t>
   </si>
   <si>
@@ -197,6 +200,15 @@
   </si>
   <si>
     <t>Astrophotography always-on button</t>
+  </si>
+  <si>
+    <t>Android 9 support?</t>
+  </si>
+  <si>
+    <t>Non-Pixel support?</t>
+  </si>
+  <si>
+    <t>BASIC</t>
   </si>
 </sst>
 </file>
@@ -218,7 +230,7 @@
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;????_);_(@_)"/>
     <numFmt numFmtId="9" formatCode="0%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -226,7 +238,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573968809" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574055446" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -241,7 +253,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573968809" fgClr="FF9900" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574055446" fgClr="FF9900" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -257,7 +269,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573968809" fgClr="999999" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574055446" fgClr="999999" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="200" lang="default" i="1"/>
@@ -272,7 +284,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573968809" fgClr="0070C0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574055446" fgClr="0070C0" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -287,7 +299,22 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1573968809" fgClr="963634" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574055446" fgClr="963634" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574055446" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -296,15 +323,26 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1574055446" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -320,7 +358,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1573968809"/>
+          <pm:border xmlns:pm="smNativeData" id="1574055446"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1574055446"/>
         </ext>
       </extLst>
     </border>
@@ -333,7 +390,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2"/>
@@ -344,6 +401,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -356,10 +414,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1573968809" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1574055446" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1573968809" count="3">
+      <pm:colors xmlns:pm="smNativeData" id="1574055446" count="3">
         <pm:color name="Color 24" rgb="FF9900"/>
         <pm:color name="Color 25" rgb="0070C0"/>
         <pm:color name="Color 26" rgb="963634"/>
@@ -625,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.144144" defaultRowHeight="13.45"/>
@@ -1121,19 +1179,49 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="10" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>38</v>
@@ -1153,7 +1241,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>38</v>
@@ -1173,7 +1261,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>38</v>
@@ -1193,7 +1281,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>38</v>
@@ -1213,7 +1301,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>38</v>
@@ -1233,12 +1321,12 @@
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>38</v>
@@ -1258,7 +1346,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>38</v>
@@ -1278,7 +1366,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>38</v>
@@ -1298,7 +1386,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>38</v>
@@ -1318,7 +1406,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>38</v>
@@ -1338,7 +1426,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>38</v>
@@ -1358,7 +1446,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>16</v>
@@ -1378,7 +1466,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>38</v>
@@ -1396,11 +1484,28 @@
         <v>38</v>
       </c>
     </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+  </mergeCells>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1573968809" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1574055446" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1409,16 +1514,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1573968809" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1573968809" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1573968809" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1573968809" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1574055446" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1574055446" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1574055446" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1574055446" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1573968809" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1574055446" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
notGoogle: maybe it wasn't going to the right config before
</commit_message>
<xml_diff>
--- a/TO DO.xlsx
+++ b/TO DO.xlsx
@@ -13,10 +13,10 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1574388431" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1574388431" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1574388431" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1574388431"/>
+      <pm:revision xmlns:pm="smNativeData" day="1574390171" val="973" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1574390171" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1574390171" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1574390171"/>
     </ext>
   </extLst>
 </workbook>
@@ -235,7 +235,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1574388431" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574390171" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -251,7 +251,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1574388431" fgClr="999999" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574390171" fgClr="999999" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="200" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="200" lang="default" i="1"/>
@@ -266,7 +266,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1574388431" fgClr="0070C0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574390171" fgClr="0070C0" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -281,7 +281,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1574388431" fgClr="963634" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574390171" fgClr="963634" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -296,7 +296,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1574388431" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1574390171" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -305,7 +305,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,19 +315,8 @@
     <fill>
       <patternFill patternType="none"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1574388431" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -343,7 +332,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1574388431"/>
+          <pm:border xmlns:pm="smNativeData" id="1574390171"/>
         </ext>
       </extLst>
     </border>
@@ -362,31 +351,12 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1574388431">
+          <pm:border xmlns:pm="smNativeData" id="1574390171">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
           </pm:border>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1574388431"/>
         </ext>
       </extLst>
     </border>
@@ -426,10 +396,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1574388431" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1574390171" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1574388431" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1574390171" count="2">
         <pm:color name="Color 24" rgb="0070C0"/>
         <pm:color name="Color 25" rgb="963634"/>
       </pm:colors>
@@ -697,7 +667,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" topLeftCell="A7" zoomScale="80" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.144144" defaultRowHeight="13.45"/>
@@ -1007,11 +977,11 @@
       <c r="B23" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>27</v>
@@ -1582,7 +1552,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1574388431" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1574390171" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1591,16 +1561,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1574388431" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1574388431" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1574388431" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1574388431" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1574390171" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1574390171" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1574390171" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1574390171" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1574388431" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1574390171" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>